<commit_message>
positive top 5 dash table implemented
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D127"/>
+  <dimension ref="A1:D214"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -452,11 +452,11 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>52</v>
+        <v>69</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Resilience amidst greater volatility Strong execution Easing of Mobility recovery in in strong growth for Gradual of in providing to our business bouncing back strongly Business</t>
+          <t>ne a altar value from any applicable and fee the peri Strong focus on improving unit economics total as a Segment proportion of</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -470,29 +470,29 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>strong growth increase growth trajectory YoY Now in</t>
+          <t>Comparison between a cohort of in e and with an active loan relative to in the same without an active loan</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Neutral</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>1</v>
+        <v>0.9999994039535522</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>64</v>
+        <v>40</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Me Vaccination Rate incremental Vaccination Rate as of Vaccination rate both partially and fully WID WHO as of Business Update Strengthening our leadership team</t>
+          <t>We believe these metrics capture significant in our business over time</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -501,16 +501,16 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>0.9999992847442627</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>117</v>
+        <v>60</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Financial Grab increasing its ownership of is a leading in Open ecosystem with a wide range of acceptance Strong potential to be the most widely accepted platform</t>
+          <t>Mobility Mobility demand to recover Mobility Initial wave of COVID Mobility grew</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -519,106 +519,106 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>1</v>
+        <v>0.9999988079071045</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>115</v>
+        <v>165</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Listing Process Update strategy Strong growth outlook across Value and convenience via Food Delivery Daily through Private</t>
+          <t>We calculate constant currency by our current period financial the corresponding prior monthly exchange for our other than the U</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Neutral</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>1</v>
+        <v>0.9999985694885254</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>48</v>
+        <v>159</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Our Key Business Winning hearts Invest for growth Reduce cost to serve Further strengthen our category Continue to drive growth across Rapidly expand our ecosystem with position across our key our core our</t>
+          <t>We calculate constant currency by our current period financial the corresponding prior monthly exchange for our other than the U</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Neutral</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>0.9999998807907104</v>
+        <v>0.9999985694885254</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>119</v>
+        <v>151</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>training by Grab Tech for Good Institute Driving thought leadership in Southeast Tech for Good Institute to drive positive impact of tech on society Thought leadership platform for the and private sector Our Key Business Winning hearts Invest for growth Reduce cost to serve Further strengthen our category Continue to drive growth across Rapidly expand our ecosystem with position across our key our core our flywheel Reconciliation to Net Loss Reconciliation S in Reconciling Interest expense from</t>
+          <t>We calculate constant currency by our current period financial the corresponding prior monthly exchange for our other than the U</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Neutral</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>0.9999997615814209</v>
+        <v>0.9999985694885254</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>49</v>
+        <v>23</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>flywheel BUSINESS resilient growth in Gross Merchandise</t>
+          <t>We calculate constant currency by our current period financial the corresponding prior monthly exchange for our other than the U</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Neutral</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>0.9999996423721313</v>
+        <v>0.9999985694885254</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>42</v>
+        <v>144</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>We believe these metrics capture significant in our business over time</t>
+          <t>We calculate constant currency by our current period financial the corresponding prior monthly exchange for our other than the U</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Neutral</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.9999992847442627</v>
+        <v>0.9999985694885254</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>57</v>
+        <v>176</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Monthly over a quarterly or annual period are calculated based on the average of the for each month in the relevant period</t>
+          <t>We calculate constant currency by our current period financial the corresponding prior monthly exchange for our other than the U</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -632,11 +632,11 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>69</v>
+        <v>96</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>over a quarterly or annual period are calculated based on the average of the for each month in the relevant period</t>
+          <t>We calculate constant currency by our current period financial the corresponding prior monthly exchange for our other than the U</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -645,16 +645,16 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>0.9999980926513672</v>
+        <v>0.9999985694885254</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>43</v>
+        <v>137</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Industry and Market Data This Presentation also and other statistical data derived from third party or some of which are preliminary by third information provided by industry or general</t>
+          <t>We calculate constant currency by our current period financial the corresponding prior monthly exchange for our other than the U</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -663,16 +663,16 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>0.9999970197677612</v>
+        <v>0.9999985694885254</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>17</v>
+        <v>100</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Use of Historical Financial Information and Financial The unaudited selected financial data for the three ended and included in this Presentation is based on financial data derived from the management that have not been or and are subject to further review and</t>
+          <t>Monthly over a quarterly or annual period are calculated based on the average of the for each month in the relevant period</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -681,16 +681,16 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>0.9999954700469971</v>
+        <v>0.9999985694885254</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>98</v>
+        <v>131</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Segment is a financial the of each of our four business in each regional corporate</t>
+          <t>We calculate constant currency by our current period financial the corresponding prior monthly exchange for our other than the U</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -699,16 +699,16 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>0.9999947547912598</v>
+        <v>0.9999985694885254</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>111</v>
+        <v>51</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Segment is a financial the of each of our four business in each regional corporate</t>
+          <t>Monthly over a quarterly or annual period are calculated based on the average of the for each month in the relevant period</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -717,16 +717,16 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>0.9999947547912598</v>
+        <v>0.9999985694885254</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>105</v>
+        <v>41</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Segment is a financial the of each of our four business in each regional corporate</t>
+          <t>Industry and Market Data This Presentation also and other statistical data derived from third party or some of which are preliminary by third information provided by industry or general</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -735,16 +735,16 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>0.9999947547912598</v>
+        <v>0.9999970197677612</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>91</v>
+        <v>26</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Segment is a financial the of each of our four business in each regional corporate</t>
+          <t>Segment is financial the of each of our four business in each regional corporate</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -753,34 +753,34 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>0.9999947547912598</v>
+        <v>0.9999959468841553</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>20</v>
+        <v>92</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>This Presentation also to financial and operating metrics</t>
+          <t>per Partner Consumer Financial Revenue Loss for the period Total Segment our for and would be</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Negative</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>0.9999945163726807</v>
+        <v>0.9999957084655762</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>58</v>
+        <v>87</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>is based on Group in which are constant since</t>
+          <t>Percentage of active in and with an active loan as of May</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -789,16 +789,16 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>0.9999934434890747</v>
+        <v>0.9999957084655762</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>29</v>
+        <v>206</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>useful information to as it the amount of a spend that is being directed through platform</t>
+          <t>l ing Food Mart Express Transport Balance Use SAM</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -807,16 +807,16 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>0.9999927282333374</v>
+        <v>0.9999948740005493</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>24</v>
+        <v>173</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>With respect to the financial we provide specific information regarding the from these financial and these financial together with their relevant financial in accordance with</t>
+          <t>Segment is a financial the of each of our four business in each regional corporate</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -825,16 +825,16 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>0.99998939037323</v>
+        <v>0.9999947547912598</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>30</v>
+        <v>162</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>This metric Grab and to evaluate and compare the total amount of customer spending that is being directed through its platform over a period of time</t>
+          <t>Segment is a financial the of each of our four business in each regional corporate</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -843,16 +843,16 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>0.9999890327453613</v>
+        <v>0.9999947547912598</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>The Company not independently such third party and no representation as to the accuracy such third party information</t>
+          <t>Commission Rate the total dollar value to Grab in the form of and from each without any for to and or to as a percentage of over the period of measurement</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -861,16 +861,16 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>0.9999881982803345</v>
+        <v>0.9999947547912598</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>4</v>
+        <v>148</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Some of these can be by the use of or other similar</t>
+          <t>Segment is a financial the of each of our four business in each regional corporate</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -879,16 +879,16 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>0.9999873638153076</v>
+        <v>0.9999947547912598</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
-        <v>14</v>
+        <v>205</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>All information provided in this Presentation is as of the date of this Presentation and any herein are based on that the Company to be reasonable as of this date</t>
+          <t>Segment is a financial the of each of our four business in each regional corporate</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -897,16 +897,16 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>0.9999862909317017</v>
+        <v>0.9999947547912598</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
-        <v>25</v>
+        <v>134</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>This Presentation also data that does not reflect elimination of intragroup which such data earnings and other from between within the Company group that are upon consolidation</t>
+          <t>Segment is a financial the of each of our four business in each regional corporate</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -915,16 +915,16 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>0.9999837875366211</v>
+        <v>0.9999947547912598</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>monthly which is defined as the monthly number of unique who transact via where transact to have successfully for any of</t>
+          <t>Segment is a financial the of each of our four business in each regional corporate</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -933,16 +933,16 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>0.9999803304672241</v>
+        <v>0.9999947547912598</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
-        <v>116</v>
+        <v>66</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Penetration rate in Across SE TAM by Penetration rate in</t>
+          <t>Segment is financial ing the of each of a in each regional corporate</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -951,16 +951,16 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>0.9999802112579346</v>
+        <v>0.9999940395355225</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
-        <v>34</v>
+        <v>212</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Gross is an operating the total dollar value to Grab in the form of and from each without any for to and or to over the period of measurement</t>
+          <t>Amount less than million a are based on unaudited</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -969,16 +969,16 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>0.9999771118164062</v>
+        <v>0.9999936819076538</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
-        <v>70</v>
+        <v>30</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Gross is an operating the total dollar value to Grab in the form of and from each without any for to and or to over the period of measurement</t>
+          <t>useful information to as it the amount of a spend that is being directed through platform</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -987,16 +987,16 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>0.9999771118164062</v>
+        <v>0.9999927282333374</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
-        <v>110</v>
+        <v>204</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Gross is an operating the total dollar value to Grab in the form of and from each without any for to and or to over the period of measurement</t>
+          <t>taking into consideration the translational to date</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1005,52 +1005,52 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>0.9999771118164062</v>
+        <v>0.9999924898147583</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
-        <v>104</v>
+        <v>44</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Gross is an operating the total dollar value to Grab in the form of and from each without any for to and or to over the period of measurement</t>
+          <t>Business Update Financial Outlook Reconciliation Driving sustainable growth in Gross Merchandise Value per Monthly YoY</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Positive</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>0.9999771118164062</v>
+        <v>0.999991774559021</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
-        <v>90</v>
+        <v>48</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Gross is an operating the total dollar value to Grab in the form of and from each without any for to and or to over the period of measurement</t>
+          <t>continue to improve in split by number of</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Positive</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>0.9999771118164062</v>
+        <v>0.9999916553497314</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
-        <v>97</v>
+        <v>11</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Gross is an operating the total dollar value to Grab in the form of and from each without any for to and or to over the period of measurement</t>
+          <t>Unaudited Financial Information and Financial unaudited selected financial data for the three ended June and included in this presentation and the investor is based on financial data derived from the management that have not been or</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1059,16 +1059,16 @@
         </is>
       </c>
       <c r="D35" t="n">
-        <v>0.9999771118164062</v>
+        <v>0.9999909400939941</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
-        <v>103</v>
+        <v>115</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>this segment data earnings and other from between within the Grab group that are upon consolidation</t>
+          <t>Commission Rate is an operating the total dollar value to Grab in the form of and from each without any for to and or to as a percentage of over the period of measurement</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1077,16 +1077,16 @@
         </is>
       </c>
       <c r="D36" t="n">
-        <v>0.9999762773513794</v>
+        <v>0.9999908208847046</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
-        <v>21</v>
+        <v>142</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Such and operating metrics should be considered only as supplemental and not as superior financial prepared in accordance with and such and operating metrics may be different from financial and operating metrics used by other</t>
+          <t>Commission Rate is an operating the total dollar value to Grab in the form of and from each without any for to and or to as a percentage of over the period of measurement</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1095,16 +1095,16 @@
         </is>
       </c>
       <c r="D37" t="n">
-        <v>0.9999752044677734</v>
+        <v>0.9999908208847046</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
-        <v>96</v>
+        <v>157</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>gross merchandise an operating metric the sum of the total dollar value of from any applicable and over the period of measurement</t>
+          <t>Commission Rate is an operating the total dollar value to Grab in the form of and from each without any for to and or to as a percentage of over the period of measurement</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1113,16 +1113,16 @@
         </is>
       </c>
       <c r="D38" t="n">
-        <v>0.9999668598175049</v>
+        <v>0.9999908208847046</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
-        <v>109</v>
+        <v>129</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>gross merchandise an operating metric the sum of the total dollar value of from any applicable and over the period of measurement</t>
+          <t>Commission Rate is an operating the total dollar value to Grab in the form of and from each without any for to and or to as a percentage of over the period of measurement</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1131,16 +1131,16 @@
         </is>
       </c>
       <c r="D39" t="n">
-        <v>0.9999668598175049</v>
+        <v>0.9999908208847046</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
-        <v>67</v>
+        <v>31</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>gross merchandise an operating metric the sum of the total dollar value of from any applicable and over the period of measurement</t>
+          <t>This metric Grab and to evaluate and compare the total amount of customer spending that is being directed through its platform over a period of time</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -1149,16 +1149,16 @@
         </is>
       </c>
       <c r="D40" t="n">
-        <v>0.9999668598175049</v>
+        <v>0.9999890327453613</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
-        <v>89</v>
+        <v>4</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>gross merchandise an operating metric the sum of the total dollar value of from any applicable and over the period of measurement</t>
+          <t>Some of these can be by the use of or other similar</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -1167,16 +1167,16 @@
         </is>
       </c>
       <c r="D41" t="n">
-        <v>0.9999668598175049</v>
+        <v>0.9999873638153076</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
-        <v>85</v>
+        <v>12</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>These are unaudited</t>
+          <t>This presentation and the investor also include to financial which Total Segment and Segment</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -1185,16 +1185,16 @@
         </is>
       </c>
       <c r="D42" t="n">
-        <v>0.9999667406082153</v>
+        <v>0.9999855756759644</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
-        <v>65</v>
+        <v>125</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Tan Ling Tan Ming Peter Chin Yin President Chief Financial Officer Chief People Officer Chief Operating Officer</t>
+          <t>Cash Liquidity cash on time marketable and restricted cash Gross Merchandise Value Commission of YOY</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -1203,16 +1203,16 @@
         </is>
       </c>
       <c r="D43" t="n">
-        <v>0.999962329864502</v>
+        <v>0.9999853372573853</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
-        <v>18</v>
+        <v>94</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>The currency is the U</t>
+          <t>million and per would be and respectively</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -1221,16 +1221,16 @@
         </is>
       </c>
       <c r="D44" t="n">
-        <v>0.9999610185623169</v>
+        <v>0.9999825954437256</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Disclaimer Operating Metrics Gross Merchandise Value is an operating metric the sum of the total dollar value of from any applicable and over the period of measurement</t>
+          <t>This presentation and the investor also data that does not reflect elimination of intragroup which such data earnings and other from between within the Grab group that are upon consolidation</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -1239,16 +1239,16 @@
         </is>
       </c>
       <c r="D45" t="n">
-        <v>0.9999544620513916</v>
+        <v>0.9999823570251465</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
-        <v>32</v>
+        <v>153</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Monthly User is defined as the monthly which is an operating metric defined as the monthly number of unique who transact via where transact to have successfully for any of</t>
+          <t>Financial Total Volume Commission of YoY</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -1257,16 +1257,16 @@
         </is>
       </c>
       <c r="D46" t="n">
-        <v>0.9999498128890991</v>
+        <v>0.9999802112579346</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
-        <v>15</v>
+        <v>90</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Undue reliance should not be on the in this which are based on information available to the Company on the date hereof</t>
+          <t>Cohort period from and August and for Financial Consolidated group</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -1275,16 +1275,16 @@
         </is>
       </c>
       <c r="D47" t="n">
-        <v>0.9999442100524902</v>
+        <v>0.999977707862854</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
-        <v>56</v>
+        <v>86</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>is defined as the monthly number of unique who transact via where transact to have successfully for any of</t>
+          <t>For the and after of first usage</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -1293,16 +1293,16 @@
         </is>
       </c>
       <c r="D48" t="n">
-        <v>0.9999401569366455</v>
+        <v>0.9999773502349854</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
-        <v>6</v>
+        <v>156</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Any such or set forth in this Presentation should be as preliminary and for illustrative only and should not be upon as being necessarily indicative of future</t>
+          <t>this segment data earnings and other from between within the Grab group that are upon consolidation</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -1311,16 +1311,16 @@
         </is>
       </c>
       <c r="D49" t="n">
-        <v>0.9999363422393799</v>
+        <v>0.9999762773513794</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
-        <v>73</v>
+        <v>196</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Total Segment is defined as the excluding regional corporate</t>
+          <t>this segment data earnings and other from between within the Grab group that are upon consolidation</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -1329,16 +1329,16 @@
         </is>
       </c>
       <c r="D50" t="n">
-        <v>0.999935507774353</v>
+        <v>0.9999762773513794</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Total Segment is defined as the excluding regional corporate</t>
+          <t>Unaudited for and</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -1347,16 +1347,16 @@
         </is>
       </c>
       <c r="D51" t="n">
-        <v>0.999935507774353</v>
+        <v>0.9999758005142212</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
-        <v>36</v>
+        <v>123</v>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>This metric Grab and to evaluate and compare the total dollar value of and by Grab over a period of time</t>
+          <t>Unaudited for and</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -1365,16 +1365,16 @@
         </is>
       </c>
       <c r="D52" t="n">
-        <v>0.9999340772628784</v>
+        <v>0.9999758005142212</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
-        <v>38</v>
+        <v>114</v>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Partner is an operating metric the dollar value of to and</t>
+          <t>Unaudited for and</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -1383,34 +1383,34 @@
         </is>
       </c>
       <c r="D53" t="n">
-        <v>0.9999299049377441</v>
+        <v>0.9999758005142212</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
-        <v>94</v>
+        <v>47</v>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Mobility Gross Merchandise Value Gross Segment</t>
+          <t>while user engagement also recovery in Mobility demand</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Positive</t>
         </is>
       </c>
       <c r="D54" t="n">
-        <v>0.9999284744262695</v>
+        <v>0.9999750852584839</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Consumer is an operating metric the dollar value of and to</t>
+          <t>We compare the percent change in our current period from the corresponding prior period constant currency</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -1419,16 +1419,16 @@
         </is>
       </c>
       <c r="D55" t="n">
-        <v>0.9999160766601562</v>
+        <v>0.9999741315841675</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Gross Merchandise Value Gross Segment</t>
+          <t>Comparison post adoption period</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -1437,16 +1437,16 @@
         </is>
       </c>
       <c r="D56" t="n">
-        <v>0.9999092817306519</v>
+        <v>0.999969482421875</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
-        <v>113</v>
+        <v>59</v>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Revenue by segment</t>
+          <t>gross merchandise an operating metric the sum of the total dollar value of from any applicable and over the period of measurement</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -1455,16 +1455,16 @@
         </is>
       </c>
       <c r="D57" t="n">
-        <v>0.999907374382019</v>
+        <v>0.9999668598175049</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
-        <v>44</v>
+        <v>98</v>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Such information a number of and and due to the nature of the and used in market cannot guarantee the accuracy of such information</t>
+          <t>gross merchandise an operating metric the sum of the total dollar value of from any applicable and over the period of measurement</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -1473,16 +1473,16 @@
         </is>
       </c>
       <c r="D58" t="n">
-        <v>0.9999046325683594</v>
+        <v>0.9999668598175049</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
-        <v>5</v>
+        <v>77</v>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>All are based upon and and reflect the and of the Company as of the date of this and may without in general economic as a result of all of which are accordingly subject to change</t>
+          <t>gross merchandise an operating metric the sum of the total dollar value of from any applicable and over the period of measurement</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -1491,16 +1491,16 @@
         </is>
       </c>
       <c r="D59" t="n">
-        <v>0.9998998641967773</v>
+        <v>0.9999668598175049</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
-        <v>86</v>
+        <v>201</v>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Cash Liquidity cash on time marketable and restricted cash</t>
+          <t>gross merchandise an operating metric the sum of the total dollar value of from any applicable and over the period of measurement</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -1509,16 +1509,16 @@
         </is>
       </c>
       <c r="D60" t="n">
-        <v>0.999886155128479</v>
+        <v>0.9999668598175049</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
-        <v>77</v>
+        <v>194</v>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Corporate cost As of</t>
+          <t>gross merchandise an operating metric the sum of the total dollar value of from any applicable and over the period of measurement</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -1527,16 +1527,16 @@
         </is>
       </c>
       <c r="D61" t="n">
-        <v>0.9998675584793091</v>
+        <v>0.9999668598175049</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
-        <v>118</v>
+        <v>141</v>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>x Grab Advancing digital Provide millions with access to bespoke training from x Grab In</t>
+          <t>gross merchandise an operating metric the sum of the total dollar value of from any applicable and over the period of measurement</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -1545,16 +1545,16 @@
         </is>
       </c>
       <c r="D62" t="n">
-        <v>0.9998666048049927</v>
+        <v>0.9999668598175049</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
-        <v>72</v>
+        <v>128</v>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Total Segment</t>
+          <t>gross merchandise an operating metric the sum of the total dollar value of from any applicable and over the period of measurement</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -1563,34 +1563,34 @@
         </is>
       </c>
       <c r="D63" t="n">
-        <v>0.9998286962509155</v>
+        <v>0.9999668598175049</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
-        <v>63</v>
+        <v>172</v>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Gradual easing of Gradual easing of a</t>
+          <t>gross merchandise an operating metric the sum of the total dollar value of from any applicable and over the period of measurement</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Neutral</t>
         </is>
       </c>
       <c r="D64" t="n">
-        <v>0.9998117089271545</v>
+        <v>0.9999668598175049</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
-        <v>13</v>
+        <v>139</v>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>It is not possible to predict all nor assess the impact of all on the business or the extent to which any or combination of may cause the actual performance or financial condition to be materially different from the of future performance of financial condition</t>
+          <t>Gross Merchandise Value Commission of YoY</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -1599,16 +1599,16 @@
         </is>
       </c>
       <c r="D65" t="n">
-        <v>0.9997883439064026</v>
+        <v>0.9999638795852661</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
-        <v>60</v>
+        <v>18</v>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>beginning Group</t>
+          <t>In light of these we provide specific information regarding the from these financial and evaluate these financial together with their relevant financial in accordance with</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -1617,16 +1617,16 @@
         </is>
       </c>
       <c r="D66" t="n">
-        <v>0.99977046251297</v>
+        <v>0.9999570846557617</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
-        <v>9</v>
+        <v>43</v>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>to the registration statement on Form with the U</t>
+          <t>Grab not independently such and no representation as to the accuracy of such information</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -1635,16 +1635,16 @@
         </is>
       </c>
       <c r="D67" t="n">
-        <v>0.9997202754020691</v>
+        <v>0.9999563694000244</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
-        <v>50</v>
+        <v>28</v>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Gross Merchandise Value</t>
+          <t>DISCLaIMer Operating Metrics Gross Merchandise Value is an operating metric the sum of the total dollar value of from any applicable and over the period of measurement</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -1653,16 +1653,16 @@
         </is>
       </c>
       <c r="D68" t="n">
-        <v>0.9997180104255676</v>
+        <v>0.9999544620513916</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
-        <v>102</v>
+        <v>63</v>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Total Volume is defined as the value of net of payment successfully through the Grab platform for the financial segment</t>
+          <t>gross merchandise an operating metric the sum of the total dollar value of from any applicable and over the period of measurement Mobility Recovery in Mobility Mobility Segment Segment as a of Mobility Segment at</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -1671,16 +1671,16 @@
         </is>
       </c>
       <c r="D69" t="n">
-        <v>0.9996757507324219</v>
+        <v>0.9999510049819946</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
-        <v>75</v>
+        <v>33</v>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>These are financial</t>
+          <t>Monthly User is defined as the monthly which is an operating metric defined as the monthly number of unique who transact via where transact to have successfully for any of</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -1689,16 +1689,16 @@
         </is>
       </c>
       <c r="D70" t="n">
-        <v>0.9996156692504883</v>
+        <v>0.9999498128890991</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
-        <v>82</v>
+        <v>9</v>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>These are financial</t>
+          <t>speak only as of the date they are made</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -1707,16 +1707,16 @@
         </is>
       </c>
       <c r="D71" t="n">
-        <v>0.9996156692504883</v>
+        <v>0.9999430179595947</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
-        <v>55</v>
+        <v>22</v>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Group Group Group</t>
+          <t>We present constant currency growth rate information to provide a framework for how our underlying and revenue excluding the effect of foreign currency rate</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -1725,16 +1725,16 @@
         </is>
       </c>
       <c r="D72" t="n">
-        <v>0.9996140599250793</v>
+        <v>0.9999380111694336</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
-        <v>23</v>
+        <v>118</v>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>There are a number of related to the use of financial and operating metrics</t>
+          <t>Total Segment is defined as the excluding regional corporate</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -1743,16 +1743,16 @@
         </is>
       </c>
       <c r="D73" t="n">
-        <v>0.999606192111969</v>
+        <v>0.999935507774353</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="n">
-        <v>26</v>
+        <v>81</v>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Such data materially from the corresponding of</t>
+          <t>more likely to use of active have an e a second Grab product than Cash active loan from Grab</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -1761,16 +1761,16 @@
         </is>
       </c>
       <c r="D74" t="n">
-        <v>0.9994956254959106</v>
+        <v>0.9999353885650635</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="n">
-        <v>39</v>
+        <v>122</v>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>The to and include base and excess with base being the amount of to and up to the amount of and by Grab from those and and excess being the amount of made to and that exceed the amount of and by Grab from those and</t>
+          <t>Net Cash Liquidity As of June As of Mar As of in unless otherwise stated Cash cash Other Time Cash Restricted cash Cash Liquidity and Net Cash Liquidity</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -1779,16 +1779,16 @@
         </is>
       </c>
       <c r="D75" t="n">
-        <v>0.9994476437568665</v>
+        <v>0.9999344348907471</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="n">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>is a metric by which Grab and its and management is necessary for to understand and evaluate its business</t>
+          <t>Partner is an operating metric the dollar value of to and</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -1797,16 +1797,16 @@
         </is>
       </c>
       <c r="D76" t="n">
-        <v>0.9993971586227417</v>
+        <v>0.9999299049377441</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="n">
-        <v>28</v>
+        <v>73</v>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>is a metric by which Grab and its and management is necessary for to understand and evaluate its business</t>
+          <t>Partner is an operating metric the dollar value of to and</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -1815,34 +1815,34 @@
         </is>
       </c>
       <c r="D77" t="n">
-        <v>0.9993971586227417</v>
+        <v>0.9999299049377441</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="n">
-        <v>59</v>
+        <v>101</v>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Business Mobility recovery as ease Mobility Growth beginning</t>
+          <t>Partner is an operating metric the dollar value of to and</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Neutral</t>
         </is>
       </c>
       <c r="D78" t="n">
-        <v>0.9992998838424683</v>
+        <v>0.9999299049377441</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="n">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Consolidated group</t>
+          <t>Partner is an operating metric the dollar value of to and</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -1851,16 +1851,16 @@
         </is>
       </c>
       <c r="D79" t="n">
-        <v>0.9992031455039978</v>
+        <v>0.9999299049377441</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="n">
-        <v>35</v>
+        <v>133</v>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Gross is a metric by which Grab and its and management is necessary for to understand and evaluate its business</t>
+          <t>Revenue YOY YoY include from Grocer Segment</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -1869,16 +1869,16 @@
         </is>
       </c>
       <c r="D80" t="n">
-        <v>0.9989181756973267</v>
+        <v>0.9999268054962158</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="n">
-        <v>101</v>
+        <v>150</v>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Mi Gross YOY Segment Of</t>
+          <t>for Constant Currency</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
@@ -1887,16 +1887,16 @@
         </is>
       </c>
       <c r="D81" t="n">
-        <v>0.998815655708313</v>
+        <v>0.9999246597290039</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="n">
-        <v>120</v>
+        <v>202</v>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Depreciation and amortization expense</t>
+          <t>for Constant Currency</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
@@ -1905,16 +1905,16 @@
         </is>
       </c>
       <c r="D82" t="n">
-        <v>0.9987651109695435</v>
+        <v>0.9999246597290039</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="n">
-        <v>41</v>
+        <v>175</v>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Partner and consumer are metrics by which we evaluate and manage our and we believe are necessary for to understand and evaluate our business</t>
+          <t>for Constant Currency</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
@@ -1923,16 +1923,16 @@
         </is>
       </c>
       <c r="D83" t="n">
-        <v>0.9987159967422485</v>
+        <v>0.9999246597290039</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="n">
-        <v>81</v>
+        <v>158</v>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>is defined as net loss to net interest income other income income tax depreciation and compensation related to and unrealized foreign exchange gain impairment on goodwill and fair value on and tax and regulatory settlement</t>
+          <t>for Constant Currency</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
@@ -1941,16 +1941,16 @@
         </is>
       </c>
       <c r="D84" t="n">
-        <v>0.9984984397888184</v>
+        <v>0.9999246597290039</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="1" t="n">
-        <v>74</v>
+        <v>143</v>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>is defined as net loss to net interest income other income income tax depreciation and compensation related to and unrealized foreign exchange gain impairment on goodwill and fair value on and tax and regulatory settlement</t>
+          <t>for Constant Currency</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
@@ -1959,16 +1959,16 @@
         </is>
       </c>
       <c r="D85" t="n">
-        <v>0.9984984397888184</v>
+        <v>0.9999246597290039</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="1" t="n">
-        <v>53</v>
+        <v>130</v>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>Mobility erased by Mobility index Sharp recovery entering to Week Beginning Business Monthly impacted by Monthly millions</t>
+          <t>for Constant Currency</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
@@ -1977,16 +1977,16 @@
         </is>
       </c>
       <c r="D86" t="n">
-        <v>0.9980416297912598</v>
+        <v>0.9999246597290039</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="1" t="n">
-        <v>107</v>
+        <v>164</v>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>Enterprise and New Gross Merchandise Gross Segment YOY YoY</t>
+          <t>for Constant Currency</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
@@ -1995,16 +1995,16 @@
         </is>
       </c>
       <c r="D87" t="n">
-        <v>0.9980400204658508</v>
+        <v>0.9999246597290039</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="1" t="n">
-        <v>7</v>
+        <v>136</v>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>The in this Presentation are subject to a number of and some of which are not currently known to the Company</t>
+          <t>for Constant Currency</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
@@ -2013,16 +2013,16 @@
         </is>
       </c>
       <c r="D88" t="n">
-        <v>0.9980267882347107</v>
+        <v>0.9999246597290039</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="1" t="n">
-        <v>83</v>
+        <v>38</v>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>For a reconciliation to the most directly comparable measure see the section titled Reconciliation</t>
+          <t>Consumer is an operating metric the dollar value of and to</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
@@ -2031,16 +2031,16 @@
         </is>
       </c>
       <c r="D89" t="n">
-        <v>0.9979845285415649</v>
+        <v>0.9999160766601562</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="1" t="n">
-        <v>112</v>
+        <v>72</v>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>For a reconciliation to the most directly comparable measure see the section titled Reconciliation</t>
+          <t>Consumer is an operating metric the dollar value of and to</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
@@ -2049,16 +2049,16 @@
         </is>
       </c>
       <c r="D90" t="n">
-        <v>0.9979845285415649</v>
+        <v>0.9999160766601562</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="1" t="n">
-        <v>76</v>
+        <v>103</v>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>For a reconciliation to the most directly comparable measure see the section titled Reconciliation</t>
+          <t>Consumer is an operating metric the dollar value of and to</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
@@ -2067,16 +2067,16 @@
         </is>
       </c>
       <c r="D91" t="n">
-        <v>0.9979845285415649</v>
+        <v>0.9999160766601562</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="1" t="n">
-        <v>92</v>
+        <v>55</v>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>For a reconciliation to the most directly comparable measure see the section titled Reconciliation</t>
+          <t>Consumer is an operating metric the dollar value of and to</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
@@ -2085,16 +2085,16 @@
         </is>
       </c>
       <c r="D92" t="n">
-        <v>0.9979845285415649</v>
+        <v>0.9999160766601562</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="1" t="n">
-        <v>106</v>
+        <v>190</v>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>For a reconciliation to the most directly comparable measure see the section titled Reconciliation</t>
+          <t>merchandise an operating metric the sum of the total dollar value from G Outlook Outlook Outlook for</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
@@ -2103,16 +2103,16 @@
         </is>
       </c>
       <c r="D93" t="n">
-        <v>0.9979845285415649</v>
+        <v>0.9999129772186279</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="1" t="n">
-        <v>99</v>
+        <v>146</v>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>For a reconciliation to the most directly comparable measure see the section titled Reconciliation</t>
+          <t>M Revenue Segment YOY of</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
@@ -2121,16 +2121,16 @@
         </is>
       </c>
       <c r="D94" t="n">
-        <v>0.9979845285415649</v>
+        <v>0.9999107122421265</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="1" t="n">
-        <v>100</v>
+        <v>54</v>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>Financial Total Volume YoY</t>
+          <t>Total include consumer and partner</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
@@ -2139,16 +2139,16 @@
         </is>
       </c>
       <c r="D95" t="n">
-        <v>0.9975553154945374</v>
+        <v>0.9999072551727295</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="1" t="n">
-        <v>19</v>
+        <v>71</v>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>dollar</t>
+          <t>Total include consumer and partner</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
@@ -2157,16 +2157,16 @@
         </is>
       </c>
       <c r="D96" t="n">
-        <v>0.9970031380653381</v>
+        <v>0.9999072551727295</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="1" t="n">
-        <v>0</v>
+        <v>99</v>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>Earnings Call Disclaimer This presentation regarding Grab</t>
+          <t>Defined as the monthly number of unique who transact via where transact to have successfully for any of</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
@@ -2175,16 +2175,16 @@
         </is>
       </c>
       <c r="D97" t="n">
-        <v>0.9968236684799194</v>
+        <v>0.9999028444290161</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="1" t="n">
-        <v>3</v>
+        <v>50</v>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>All other than of historical fact in this as to future of and financial and business strategy and of management for future of the market size and growth competitive position and technological and market are</t>
+          <t>Defined as the monthly number of unique who transact via where transact to have successfully for any of</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
@@ -2193,16 +2193,16 @@
         </is>
       </c>
       <c r="D98" t="n">
-        <v>0.9967973828315735</v>
+        <v>0.9999028444290161</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="1" t="n">
-        <v>2</v>
+        <v>203</v>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>Actual may differ materially from the and should not be considered as an indication of future performance</t>
+          <t>We estimate the variance between Constant Currency and Currency growth for in to be c</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
@@ -2211,16 +2211,16 @@
         </is>
       </c>
       <c r="D99" t="n">
-        <v>0.996529757976532</v>
+        <v>0.9999011754989624</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="1" t="n">
-        <v>125</v>
+        <v>189</v>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>Total</t>
+          <t>to made to driver Financial and and Q and Enterprise New by b and Group</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
@@ -2229,16 +2229,16 @@
         </is>
       </c>
       <c r="D100" t="n">
-        <v>0.9963483214378357</v>
+        <v>0.9998964071273804</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="1" t="n">
-        <v>66</v>
+        <v>104</v>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>Consolidated group Gross Merchandise per Monthly Gross YOY YoY YOY</t>
+          <t>Total Segment is defined as the excluding regional corporate cost</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
@@ -2247,34 +2247,34 @@
         </is>
       </c>
       <c r="D101" t="n">
-        <v>0.9960391521453857</v>
+        <v>0.999879002571106</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="1" t="n">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>Consolidated group Revenue Net Loss Cash</t>
+          <t>and productivity and satisfaction with and stickiness</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Positive</t>
         </is>
       </c>
       <c r="D102" t="n">
-        <v>0.9959238767623901</v>
+        <v>0.9998703002929688</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="1" t="n">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>The Company no duty to update this information unless by law</t>
+          <t>the presentation of these financial is not intended to be considered in isolation or as an alternative financial determined in accordance with</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
@@ -2283,16 +2283,16 @@
         </is>
       </c>
       <c r="D103" t="n">
-        <v>0.9948320388793945</v>
+        <v>0.9998549222946167</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="1" t="n">
-        <v>108</v>
+        <v>178</v>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>i YoY</t>
+          <t>In millions Base Excess Consumer Total Base Excess Consumer Total</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
@@ -2301,34 +2301,34 @@
         </is>
       </c>
       <c r="D104" t="n">
-        <v>0.9939911961555481</v>
+        <v>0.9998469352722168</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="1" t="n">
-        <v>54</v>
+        <v>27</v>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>Notwithstanding would have grown conviction in our strategy</t>
+          <t>margin is a financial measure calculated as divided by Gross Merchandise Value</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Neutral</t>
         </is>
       </c>
       <c r="D105" t="n">
-        <v>0.9936226010322571</v>
+        <v>0.9998435974121094</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="1" t="n">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>You are not to give undue weight on such</t>
+          <t>i m m offering</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
@@ -2337,16 +2337,16 @@
         </is>
       </c>
       <c r="D106" t="n">
-        <v>0.9931761622428894</v>
+        <v>0.9998210072517395</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="1" t="n">
-        <v>124</v>
+        <v>10</v>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>Enterprise New</t>
+          <t>Grab does not undertake any obligation to update any whether as a result of new future or except as under applicable law</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
@@ -2355,34 +2355,34 @@
         </is>
       </c>
       <c r="D107" t="n">
-        <v>0.9856954216957092</v>
+        <v>0.9998156428337097</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="1" t="n">
-        <v>121</v>
+        <v>16</v>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>Gift Mar Appendix on Base Excess Consumer Base Excess Consumer</t>
+          <t>For management Total Segment as a useful indicator of the economics of business as it does not include regional corporate</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>Negative</t>
+          <t>Neutral</t>
         </is>
       </c>
       <c r="D108" t="n">
-        <v>0.9850992560386658</v>
+        <v>0.9998099207878113</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="1" t="n">
-        <v>10</v>
+        <v>121</v>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>and Exchange Commission by Grab Limited on and other from time to time with the SEC</t>
+          <t>settlement and share listing and associated</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
@@ -2391,16 +2391,16 @@
         </is>
       </c>
       <c r="D109" t="n">
-        <v>0.9786873459815979</v>
+        <v>0.9997822642326355</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="1" t="n">
-        <v>62</v>
+        <v>207</v>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>Resumption of interstate travel to a Vaccination Travel Gradual easing of six a</t>
+          <t>The h S N y</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
@@ -2409,16 +2409,16 @@
         </is>
       </c>
       <c r="D110" t="n">
-        <v>0.9595246911048889</v>
+        <v>0.99977046251297</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="1" t="n">
-        <v>37</v>
+        <v>62</v>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>Grab Gross as a metric to understand and and to enable to understand and its aggregate operating which significant in its business over time</t>
+          <t>Mobility in is of</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
@@ -2427,16 +2427,16 @@
         </is>
       </c>
       <c r="D111" t="n">
-        <v>0.9394102096557617</v>
+        <v>0.9997673630714417</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="1" t="n">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>These filings identify and address other important and that could cause actual and to differ materially from those in the</t>
+          <t>Explanation of financial is a financial measure calculated as net loss to interest income other income income tax depreciation and compensation related to and unrealized foreign exchange gain impairment on goodwill and fair value on tax and regulatory settlement and share listing and associated</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
@@ -2445,16 +2445,16 @@
         </is>
       </c>
       <c r="D112" t="n">
-        <v>0.9378294944763184</v>
+        <v>0.9997419714927673</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="1" t="n">
-        <v>31</v>
+        <v>5</v>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>Grab as a metric to understand and and to enable to understand and aggregate operating which significant in its business over time</t>
+          <t>are based upon and and reflect the and of which involve inherent and and therefore should not be upon as being necessarily indicative of future</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
@@ -2463,16 +2463,16 @@
         </is>
       </c>
       <c r="D113" t="n">
-        <v>0.9287499785423279</v>
+        <v>0.9997015595436096</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="1" t="n">
-        <v>8</v>
+        <v>93</v>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>You should carefully consider the and in the section of Amendment No</t>
+          <t>million and</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
@@ -2481,16 +2481,16 @@
         </is>
       </c>
       <c r="D114" t="n">
-        <v>0.9232849478721619</v>
+        <v>0.9996935129165649</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="1" t="n">
-        <v>1</v>
+        <v>195</v>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>future business which involve and</t>
+          <t>Total Volume is defined as the value of net of payment successfully through the Grab platform for the financial segment</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
@@ -2499,16 +2499,16 @@
         </is>
       </c>
       <c r="D115" t="n">
-        <v>0.9147056341171265</v>
+        <v>0.9996757507324219</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="1" t="n">
-        <v>123</v>
+        <v>155</v>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>Financial</t>
+          <t>Total Volume is defined as the value of net of payment successfully through the Grab platform for the financial segment</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
@@ -2517,16 +2517,16 @@
         </is>
       </c>
       <c r="D116" t="n">
-        <v>0.8873853087425232</v>
+        <v>0.9996757507324219</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="1" t="n">
-        <v>88</v>
+        <v>57</v>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>YoY</t>
+          <t>The to and include base and excess with base being the amount of to and up to the number of and by Grab from those and and excess being the amount of made to and that exceed the amount of and by Grab from those and</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
@@ -2535,34 +2535,34 @@
         </is>
       </c>
       <c r="D117" t="n">
-        <v>0.8766493201255798</v>
+        <v>0.9996434450149536</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="1" t="n">
-        <v>79</v>
+        <v>53</v>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>of driven by a i Amortization Interest Expense Total Segment Regional Other Income Loss for corporate the period</t>
+          <t>as a proportion of</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>Negative</t>
+          <t>Neutral</t>
         </is>
       </c>
       <c r="D118" t="n">
-        <v>0.8671250939369202</v>
+        <v>0.9996378421783447</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="1" t="n">
-        <v>22</v>
+        <v>106</v>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>The Company these financial and operating metrics for financial and operational and as a to evaluate and the management that these financial and operating metrics provide meaningful supplemental information regarding the performance by excluding certain that may not be indicative of its recurring core business operating</t>
+          <t>These are financial</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
@@ -2571,16 +2571,16 @@
         </is>
       </c>
       <c r="D119" t="n">
-        <v>0.7704790830612183</v>
+        <v>0.9996156692504883</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="1" t="n">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>YoY YoY</t>
+          <t>gross an operating metric the sum of</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
@@ -2589,34 +2589,34 @@
         </is>
       </c>
       <c r="D120" t="n">
-        <v>0.6832816600799561</v>
+        <v>0.9995984435081482</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="1" t="n">
-        <v>61</v>
+        <v>102</v>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>gross merchandise an operating metric the sum of the total dollar value of from any applicable and over the period of measurement Business Continued with higher</t>
+          <t>The up to the amount of and by Grab from those and and excess</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Neutral</t>
         </is>
       </c>
       <c r="D121" t="n">
-        <v>0.6764038801193237</v>
+        <v>0.9995394945144653</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="1" t="n">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>Mobility</t>
+          <t>YoY Change Commission</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
@@ -2625,16 +2625,16 @@
         </is>
       </c>
       <c r="D122" t="n">
-        <v>0.6590568423271179</v>
+        <v>0.9995003938674927</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="1" t="n">
-        <v>122</v>
+        <v>20</v>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>Mobility</t>
+          <t>Such data materially from the corresponding of</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
@@ -2643,34 +2643,34 @@
         </is>
       </c>
       <c r="D123" t="n">
-        <v>0.6590568423271179</v>
+        <v>0.9994956254959106</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" s="1" t="n">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>Business Update Strategy Update Reconciliation Mart</t>
+          <t>YoY YoY Revenue Gross Merchandise Value YoY Constant</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Neutral</t>
         </is>
       </c>
       <c r="D124" t="n">
-        <v>0.6527711749076843</v>
+        <v>0.9994762539863586</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" s="1" t="n">
-        <v>12</v>
+        <v>108</v>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>the Company in a very competitive and rapidly and new may emerge from time to time</t>
+          <t>with base being the amount of to and exceed the amount of and by Grab from those and to and include base a the amount of made to and related to and unrealized foreign exchange</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
@@ -2679,16 +2679,16 @@
         </is>
       </c>
       <c r="D125" t="n">
-        <v>0.6396925449371338</v>
+        <v>0.9994695782661438</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" s="1" t="n">
-        <v>78</v>
+        <v>14</v>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>of YoY increase in</t>
+          <t>In these financial may differ from financial with comparable used by other</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
@@ -2697,16 +2697,16 @@
         </is>
       </c>
       <c r="D126" t="n">
-        <v>0.600771427154541</v>
+        <v>0.9994694590568542</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" s="1" t="n">
-        <v>95</v>
+        <v>37</v>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>YoY YOY YoY</t>
+          <t>The to and include base and excess with base being the amount of to and up to the amount of and by Grab from those and and excess being the amount of made to and that exceed the amount of and by Grab from those and</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
@@ -2715,7 +2715,1573 @@
         </is>
       </c>
       <c r="D127" t="n">
-        <v>0.5004815459251404</v>
+        <v>0.9994476437568665</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" s="1" t="n">
+        <v>74</v>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>The to and include base and excess with base being the amount of to and up to the amount of and by Grab from those and and excess being the amount of made to and that exceed the amount of and by Grab from those and</t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="D128" t="n">
+        <v>0.9994476437568665</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>Disclaimer This presentation and the investor contain within the meaning of the of the U</t>
+        </is>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="D129" t="n">
+        <v>0.9994472861289978</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" s="1" t="n">
+        <v>167</v>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>Enterprise and New Gross Merchandise</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="D130" t="n">
+        <v>0.9994062185287476</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>is a metric by which Grab and its and management is necessary for to understand and evaluate its business</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="D131" t="n">
+        <v>0.9993971586227417</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>is a metric by which Grab and its and management is necessary for to understand and evaluate its business</t>
+        </is>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="D132" t="n">
+        <v>0.9993971586227417</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" s="1" t="n">
+        <v>91</v>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>Change Change in unless otherwise stated of Operating Metrics of</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="D133" t="n">
+        <v>0.9993759989738464</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" s="1" t="n">
+        <v>184</v>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>Base Excess Consumer Total Base Excess Consumer Total</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="D134" t="n">
+        <v>0.999306321144104</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" s="1" t="n">
+        <v>199</v>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>Segment</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="D135" t="n">
+        <v>0.9992735981941223</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" s="1" t="n">
+        <v>124</v>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>For only and are but cash liquidity and net cash liquidity are not</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="D136" t="n">
+        <v>0.9991573095321655</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" s="1" t="n">
+        <v>211</v>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>tax and regulatory settlement</t>
+        </is>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="D137" t="n">
+        <v>0.9991471767425537</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" s="1" t="n">
+        <v>193</v>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>Note</t>
+        </is>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="D138" t="n">
+        <v>0.9990105628967285</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" s="1" t="n">
+        <v>208</v>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>fe to Net Loss Reconciliation Si in unless otherwise stated</t>
+        </is>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="D139" t="n">
+        <v>0.9989855885505676</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" s="1" t="n">
+        <v>78</v>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>Financial Financial user engagement</t>
+        </is>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="D140" t="n">
+        <v>0.9989631175994873</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" s="1" t="n">
+        <v>65</v>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>as omen of Mobility</t>
+        </is>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="D141" t="n">
+        <v>0.9989294409751892</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" s="1" t="n">
+        <v>127</v>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>include from Grocer</t>
+        </is>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="D142" t="n">
+        <v>0.9988628625869751</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" s="1" t="n">
+        <v>113</v>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>include from Grocer</t>
+        </is>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="D143" t="n">
+        <v>0.9988628625869751</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" s="1" t="n">
+        <v>85</v>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>those without</t>
+        </is>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="D144" t="n">
+        <v>0.9987486600875854</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>Partner and consumer are metrics by which we evaluate and manage our and we believe are necessary for to understand and evaluate our business</t>
+        </is>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="D145" t="n">
+        <v>0.9987159967422485</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>Earnings Call August</t>
+        </is>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="D146" t="n">
+        <v>0.9985389709472656</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" s="1" t="n">
+        <v>70</v>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>and include from Grocer</t>
+        </is>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="D147" t="n">
+        <v>0.9984580278396606</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>There are a number of related to the use of financial</t>
+        </is>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="D148" t="n">
+        <v>0.9983566403388977</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>and Exchange Commission</t>
+        </is>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="D149" t="n">
+        <v>0.9982213377952576</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" s="1" t="n">
+        <v>119</v>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>is defined as net loss to net interest income other income income tax depreciation and cor n related to and unrealized foreign exchange gain impairment on goodwill and fair value on tax and regulatory are financial</t>
+        </is>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="D150" t="n">
+        <v>0.9981732368469238</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>All other than of historical fact in this presentation and the but not limited about and business strategy and of management for future of and growth are</t>
+        </is>
+      </c>
+      <c r="C151" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="D151" t="n">
+        <v>0.9981427192687988</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>Such information a number of and and you are not to give undue weight on such</t>
+        </is>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="D152" t="n">
+        <v>0.998094379901886</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" s="1" t="n">
+        <v>120</v>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>For a reconciliation to the most directly comparable measure see the section titled Reconciliation</t>
+        </is>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="D153" t="n">
+        <v>0.9979845285415649</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" s="1" t="n">
+        <v>135</v>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>For a reconciliation to the most directly comparable measure see the section titled Reconciliation</t>
+        </is>
+      </c>
+      <c r="C154" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="D154" t="n">
+        <v>0.9979845285415649</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" s="1" t="n">
+        <v>163</v>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>For a reconciliation to the most directly comparable measure see the section titled Reconciliation</t>
+        </is>
+      </c>
+      <c r="C155" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="D155" t="n">
+        <v>0.9979845285415649</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" s="1" t="n">
+        <v>76</v>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>For a reconciliation to the most directly comparable measure see the section titled Reconciliation</t>
+        </is>
+      </c>
+      <c r="C156" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="D156" t="n">
+        <v>0.9979845285415649</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" s="1" t="n">
+        <v>149</v>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>For a reconciliation to the most directly comparable measure see the section titled Reconciliation</t>
+        </is>
+      </c>
+      <c r="C157" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="D157" t="n">
+        <v>0.9979845285415649</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" s="1" t="n">
+        <v>174</v>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>For a reconciliation to the most directly comparable measure see the section titled Reconciliation</t>
+        </is>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="D158" t="n">
+        <v>0.9979845285415649</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" s="1" t="n">
+        <v>58</v>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>is defined as net loss to net interest income other income income tax depreciation and compensation related to and unrealized foreign exchange gain impairment on goodwill and fair value on tax and regulatory settlement and share listing and associated</t>
+        </is>
+      </c>
+      <c r="C159" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="D159" t="n">
+        <v>0.9978583455085754</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" s="1" t="n">
+        <v>200</v>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>ore Note</t>
+        </is>
+      </c>
+      <c r="C160" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="D160" t="n">
+        <v>0.9978393316268921</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" s="1" t="n">
+        <v>107</v>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>For a reconciliation to the most directly comparable measure see the section tit Reconciliation</t>
+        </is>
+      </c>
+      <c r="C161" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="D161" t="n">
+        <v>0.9978232383728027</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" s="1" t="n">
+        <v>109</v>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>Commission</t>
+        </is>
+      </c>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="D162" t="n">
+        <v>0.997200608253479</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>dollar</t>
+        </is>
+      </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="D163" t="n">
+        <v>0.9970031380653381</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" s="1" t="n">
+        <v>166</v>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>dollar</t>
+        </is>
+      </c>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="D164" t="n">
+        <v>0.9970031380653381</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" s="1" t="n">
+        <v>177</v>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>dollar</t>
+        </is>
+      </c>
+      <c r="C165" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="D165" t="n">
+        <v>0.9970031380653381</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" s="1" t="n">
+        <v>152</v>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>dollar</t>
+        </is>
+      </c>
+      <c r="C166" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="D166" t="n">
+        <v>0.9970031380653381</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" s="1" t="n">
+        <v>160</v>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>dollar</t>
+        </is>
+      </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="D167" t="n">
+        <v>0.9970031380653381</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" s="1" t="n">
+        <v>145</v>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>dollar</t>
+        </is>
+      </c>
+      <c r="C168" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="D168" t="n">
+        <v>0.9970031380653381</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" s="1" t="n">
+        <v>138</v>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>dollar</t>
+        </is>
+      </c>
+      <c r="C169" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="D169" t="n">
+        <v>0.9970031380653381</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" s="1" t="n">
+        <v>97</v>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>dollar</t>
+        </is>
+      </c>
+      <c r="C170" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="D170" t="n">
+        <v>0.9970031380653381</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" s="1" t="n">
+        <v>132</v>
+      </c>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t>dollar</t>
+        </is>
+      </c>
+      <c r="C171" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="D171" t="n">
+        <v>0.9970031380653381</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" s="1" t="n">
+        <v>64</v>
+      </c>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t>in In line with steady state of AM</t>
+        </is>
+      </c>
+      <c r="C172" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="D172" t="n">
+        <v>0.996707022190094</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" s="1" t="n">
+        <v>188</v>
+      </c>
+      <c r="B173" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="C173" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="D173" t="n">
+        <v>0.9963483214378357</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" s="1" t="n">
+        <v>182</v>
+      </c>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="C174" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="D174" t="n">
+        <v>0.9963483214378357</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" s="1" t="n">
+        <v>183</v>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>As a of</t>
+        </is>
+      </c>
+      <c r="C175" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="D175" t="n">
+        <v>0.9963239431381226</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" s="1" t="n">
+        <v>168</v>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>Revenue Segment YoY</t>
+        </is>
+      </c>
+      <c r="C176" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="D176" t="n">
+        <v>0.9960137605667114</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" s="1" t="n">
+        <v>161</v>
+      </c>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t>Financial Revenue Segment YOY YoY</t>
+        </is>
+      </c>
+      <c r="C177" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="D177" t="n">
+        <v>0.9957798719406128</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" s="1" t="n">
+        <v>105</v>
+      </c>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t>is defined as net loss to net interest income other income income tax depreciation and compensation gain impairment on goodwill and fair value on tax and regulatory settlement and share listing and associated</t>
+        </is>
+      </c>
+      <c r="C178" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="D178" t="n">
+        <v>0.9948837161064148</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" s="1" t="n">
+        <v>67</v>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>For a to the most dirt e n titled</t>
+        </is>
+      </c>
+      <c r="C179" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="D179" t="n">
+        <v>0.9948193430900574</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" s="1" t="n">
+        <v>198</v>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>Revenue</t>
+        </is>
+      </c>
+      <c r="C180" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="D180" t="n">
+        <v>0.9907988309860229</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" s="1" t="n">
+        <v>209</v>
+      </c>
+      <c r="B181" t="inlineStr">
+        <is>
+          <t>Net interest Other income Income tax Depreciation and amortization compensation Unrealized foreign exchange</t>
+        </is>
+      </c>
+      <c r="C181" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="D181" t="n">
+        <v>0.990572988986969</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B182" t="inlineStr">
+        <is>
+          <t>In addition to the foregoing you should also carefully consider the other and in the section of registration statement on Form and the prospectus and other by Grab from time to time with the U</t>
+        </is>
+      </c>
+      <c r="C182" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="D182" t="n">
+        <v>0.9888788461685181</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" s="1" t="n">
+        <v>84</v>
+      </c>
+      <c r="B183" t="inlineStr">
+        <is>
+          <t>higher than Cash more</t>
+        </is>
+      </c>
+      <c r="C183" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="D183" t="n">
+        <v>0.9873208999633789</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" s="1" t="n">
+        <v>181</v>
+      </c>
+      <c r="B184" t="inlineStr">
+        <is>
+          <t>Enterprise New</t>
+        </is>
+      </c>
+      <c r="C184" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="D184" t="n">
+        <v>0.9856954216957092</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" s="1" t="n">
+        <v>187</v>
+      </c>
+      <c r="B185" t="inlineStr">
+        <is>
+          <t>Enterprise New</t>
+        </is>
+      </c>
+      <c r="C185" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="D185" t="n">
+        <v>0.9856954216957092</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" s="1" t="n">
+        <v>197</v>
+      </c>
+      <c r="B186" t="inlineStr">
+        <is>
+          <t>Outlook Outlook for and YoY growth YoY</t>
+        </is>
+      </c>
+      <c r="C186" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="D186" t="n">
+        <v>0.9856483936309814</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" s="1" t="n">
+        <v>210</v>
+      </c>
+      <c r="B187" t="inlineStr">
+        <is>
+          <t>Impairment on goodwill and assets Fair value change on</t>
+        </is>
+      </c>
+      <c r="C187" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="D187" t="n">
+        <v>0.9846363067626953</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="B188" t="inlineStr">
+        <is>
+          <t>YoY Constant Currency YoY Constant Currency is defined as the monthly number of currency by our current period Business Increasing and engagement continue to driven by the</t>
+        </is>
+      </c>
+      <c r="C188" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="D188" t="n">
+        <v>0.9740327000617981</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B189" t="inlineStr">
+        <is>
+          <t>Private Litigation Reform Act of</t>
+        </is>
+      </c>
+      <c r="C189" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="D189" t="n">
+        <v>0.9730282425880432</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" s="1" t="n">
+        <v>80</v>
+      </c>
+      <c r="B190" t="inlineStr">
+        <is>
+          <t>our are</t>
+        </is>
+      </c>
+      <c r="C190" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="D190" t="n">
+        <v>0.9705395102500916</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" s="1" t="n">
+        <v>82</v>
+      </c>
+      <c r="B191" t="inlineStr">
+        <is>
+          <t>retention of</t>
+        </is>
+      </c>
+      <c r="C191" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="D191" t="n">
+        <v>0.9687386155128479</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="B192" t="inlineStr">
+        <is>
+          <t>Grab as a metric to understand and and to enable to understand and aggregate operating which significant in its business over time</t>
+        </is>
+      </c>
+      <c r="C192" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="D192" t="n">
+        <v>0.9287499785423279</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" s="1" t="n">
+        <v>170</v>
+      </c>
+      <c r="B193" t="inlineStr">
+        <is>
+          <t>YoY of</t>
+        </is>
+      </c>
+      <c r="C193" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="D193" t="n">
+        <v>0.9051330089569092</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" s="1" t="n">
+        <v>186</v>
+      </c>
+      <c r="B194" t="inlineStr">
+        <is>
+          <t>Financial</t>
+        </is>
+      </c>
+      <c r="C194" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="D194" t="n">
+        <v>0.8873854279518127</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" s="1" t="n">
+        <v>180</v>
+      </c>
+      <c r="B195" t="inlineStr">
+        <is>
+          <t>Financial</t>
+        </is>
+      </c>
+      <c r="C195" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="D195" t="n">
+        <v>0.8873854279518127</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" s="1" t="n">
+        <v>112</v>
+      </c>
+      <c r="B196" t="inlineStr">
+        <is>
+          <t>Financial</t>
+        </is>
+      </c>
+      <c r="C196" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="D196" t="n">
+        <v>0.8873854279518127</v>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" s="1" t="n">
+        <v>192</v>
+      </c>
+      <c r="B197" t="inlineStr">
+        <is>
+          <t>Financial</t>
+        </is>
+      </c>
+      <c r="C197" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="D197" t="n">
+        <v>0.8873854279518127</v>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" s="1" t="n">
+        <v>126</v>
+      </c>
+      <c r="B198" t="inlineStr">
+        <is>
+          <t>YoY</t>
+        </is>
+      </c>
+      <c r="C198" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="D198" t="n">
+        <v>0.8766494989395142</v>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" s="1" t="n">
+        <v>171</v>
+      </c>
+      <c r="B199" t="inlineStr">
+        <is>
+          <t>YoY</t>
+        </is>
+      </c>
+      <c r="C199" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="D199" t="n">
+        <v>0.8766494989395142</v>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" s="1" t="n">
+        <v>140</v>
+      </c>
+      <c r="B200" t="inlineStr">
+        <is>
+          <t>YoY</t>
+        </is>
+      </c>
+      <c r="C200" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="D200" t="n">
+        <v>0.8766494989395142</v>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" s="1" t="n">
+        <v>154</v>
+      </c>
+      <c r="B201" t="inlineStr">
+        <is>
+          <t>YoY</t>
+        </is>
+      </c>
+      <c r="C201" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="D201" t="n">
+        <v>0.8766494989395142</v>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B202" t="inlineStr">
+        <is>
+          <t>Grab these financial for financial and operational and as a to evaluate and management that these financial provide meaningful supplemental information regarding its performance by excluding certain that may not be indicative of its recurring core business operating</t>
+        </is>
+      </c>
+      <c r="C202" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="D202" t="n">
+        <v>0.8615102767944336</v>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" s="1" t="n">
+        <v>61</v>
+      </c>
+      <c r="B203" t="inlineStr">
+        <is>
+          <t>YoY and its Omicron impact highest level since impact</t>
+        </is>
+      </c>
+      <c r="C203" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="D203" t="n">
+        <v>0.8482586741447449</v>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" s="1" t="n">
+        <v>117</v>
+      </c>
+      <c r="B204" t="inlineStr">
+        <is>
+          <t>Cash Loss for the period Unaudited for and</t>
+        </is>
+      </c>
+      <c r="C204" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+      <c r="D204" t="n">
+        <v>0.7247083783149719</v>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" s="1" t="n">
+        <v>169</v>
+      </c>
+      <c r="B205" t="inlineStr">
+        <is>
+          <t>YOY YoY</t>
+        </is>
+      </c>
+      <c r="C205" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="D205" t="n">
+        <v>0.6832810044288635</v>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" s="1" t="n">
+        <v>147</v>
+      </c>
+      <c r="B206" t="inlineStr">
+        <is>
+          <t>YoY YoY</t>
+        </is>
+      </c>
+      <c r="C206" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="D206" t="n">
+        <v>0.6832810044288635</v>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" s="1" t="n">
+        <v>185</v>
+      </c>
+      <c r="B207" t="inlineStr">
+        <is>
+          <t>Mobility</t>
+        </is>
+      </c>
+      <c r="C207" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="D207" t="n">
+        <v>0.6590566635131836</v>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" s="1" t="n">
+        <v>179</v>
+      </c>
+      <c r="B208" t="inlineStr">
+        <is>
+          <t>Mobility</t>
+        </is>
+      </c>
+      <c r="C208" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="D208" t="n">
+        <v>0.6590566635131836</v>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" s="1" t="n">
+        <v>111</v>
+      </c>
+      <c r="B209" t="inlineStr">
+        <is>
+          <t>Mobility</t>
+        </is>
+      </c>
+      <c r="C209" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="D209" t="n">
+        <v>0.6590566635131836</v>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" s="1" t="n">
+        <v>191</v>
+      </c>
+      <c r="B210" t="inlineStr">
+        <is>
+          <t>Mobility</t>
+        </is>
+      </c>
+      <c r="C210" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="D210" t="n">
+        <v>0.6590566635131836</v>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B211" t="inlineStr">
+        <is>
+          <t>A number of could cause actual to differ materially from those in any but not limited ability to grow at the desired rate or scale and its ability to manage its its ability to further develop its new and its ability to attract and retain and its ability to compete effectively in the intensely competitive and constantly its ability to continue to raise sufficient its ability to reduce net and the use of partner and consumer and to achieve potential impact of the complex legal and regulatory environment on its its ability to protect and maintain its brand and general economic in particular as a result of growth of in which Grab or may and its ability to defend any legal or governmental against it</t>
+        </is>
+      </c>
+      <c r="C211" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="D211" t="n">
+        <v>0.6399646997451782</v>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" s="1" t="n">
+        <v>83</v>
+      </c>
+      <c r="B212" t="inlineStr">
+        <is>
+          <t>and with record e X are</t>
+        </is>
+      </c>
+      <c r="C212" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="D212" t="n">
+        <v>0.6343331336975098</v>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" s="1" t="n">
+        <v>116</v>
+      </c>
+      <c r="B213" t="inlineStr">
+        <is>
+          <t>Segment to Net Loss in unless otherwise stated Total Segment Regional Corporate Regional Corporate fell from in to in</t>
+        </is>
+      </c>
+      <c r="C213" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+      <c r="D213" t="n">
+        <v>0.6111045479774475</v>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="B214" t="inlineStr">
+        <is>
+          <t>may not add up to due to rounding Business Improvement in and unit economics Total as a proportion of</t>
+        </is>
+      </c>
+      <c r="C214" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="D214" t="n">
+        <v>0.5392075181007385</v>
       </c>
     </row>
   </sheetData>

</xml_diff>